<commit_message>
Playing around with angle of pixel to make it more steep. Also changed bump so it doesn't create a narrowing of the channel. Added python script to process the csv file from Excel. I have not tried printing this. In fact, I made these changes while test #3 is printing.
</commit_message>
<xml_diff>
--- a/Labyrinth_maze.xlsx
+++ b/Labyrinth_maze.xlsx
@@ -452,7 +452,7 @@
   <dimension ref="A1:CV18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CP16" sqref="CP16"/>
+      <selection activeCell="BS12" sqref="BS12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3096,10 +3096,10 @@
         <v>0</v>
       </c>
       <c r="BT9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV9" s="1">
         <v>1</v>
@@ -3120,13 +3120,13 @@
         <v>1</v>
       </c>
       <c r="CB9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE9" s="1">
         <v>0</v>
@@ -3407,7 +3407,7 @@
         <v>0</v>
       </c>
       <c r="CA10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB10" s="1">
         <v>0</v>
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="CD10" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE10" s="1">
         <v>0</v>
@@ -3697,7 +3697,7 @@
         <v>0</v>
       </c>
       <c r="CA11" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB11" s="1">
         <v>0</v>
@@ -3706,7 +3706,7 @@
         <v>0</v>
       </c>
       <c r="CD11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE11" s="1">
         <v>0</v>
@@ -3987,7 +3987,7 @@
         <v>0</v>
       </c>
       <c r="CA12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB12" s="1">
         <v>0</v>
@@ -3996,7 +3996,7 @@
         <v>0</v>
       </c>
       <c r="CD12" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE12" s="1">
         <v>0</v>
@@ -4277,7 +4277,7 @@
         <v>0</v>
       </c>
       <c r="CA13" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB13" s="1">
         <v>0</v>
@@ -4286,7 +4286,7 @@
         <v>0</v>
       </c>
       <c r="CD13" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE13" s="1">
         <v>0</v>
@@ -4567,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="CA14" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB14" s="1">
         <v>0</v>
@@ -4576,7 +4576,7 @@
         <v>0</v>
       </c>
       <c r="CD14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE14" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Okay this is test #6. 0.2mm layer height 0.6mm lid to base gap 10 lines of puzzle. I reduced the fan-out of the pixel in an attempt to fit more puzzle in the same space. Hopefully this is not too tight.
</commit_message>
<xml_diff>
--- a/Labyrinth_maze.xlsx
+++ b/Labyrinth_maze.xlsx
@@ -18,9 +18,13 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -40,6 +44,13 @@
       <u/>
       <sz val="12"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -74,7 +85,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="69">
+  <cellStyleXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -144,8 +155,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -156,8 +177,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="69">
+  <cellStyles count="79">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -192,6 +216,11 @@
     <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -226,6 +255,11 @@
     <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -555,23 +589,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV119"/>
+  <dimension ref="A1:DH119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="Y110" sqref="Y110"/>
+    <sheetView tabSelected="1" topLeftCell="BV12" workbookViewId="0">
+      <selection activeCell="CP15" sqref="CP15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="19" width="2" style="1" customWidth="1"/>
-    <col min="20" max="94" width="2" customWidth="1"/>
-    <col min="95" max="95" width="2.5" customWidth="1"/>
-    <col min="96" max="96" width="2" customWidth="1"/>
-    <col min="97" max="99" width="2.6640625" customWidth="1"/>
-    <col min="100" max="100" width="4.5" customWidth="1"/>
+    <col min="1" max="19" width="6.5" style="1" customWidth="1"/>
+    <col min="20" max="100" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:100">
+    <row r="1" spans="1:112">
       <c r="A1" s="3">
         <v>1</v>
       </c>
@@ -972,7 +1002,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="2" spans="1:100">
+    <row r="2" spans="1:112">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -1274,7 +1304,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:100">
+    <row r="3" spans="1:112">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1576,7 +1606,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:100">
+    <row r="4" spans="1:112">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1878,7 +1908,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:100">
+    <row r="5" spans="1:112">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2180,7 +2210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:100">
+    <row r="6" spans="1:112">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -2482,7 +2512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:100">
+    <row r="7" spans="1:112">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -2784,7 +2814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:100">
+    <row r="8" spans="1:112">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -3086,7 +3116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:100">
+    <row r="9" spans="1:112">
       <c r="A9" s="1">
         <v>1</v>
       </c>
@@ -3388,7 +3418,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:100">
+    <row r="10" spans="1:112">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -3690,7 +3720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:100">
+    <row r="11" spans="1:112">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -3992,7 +4022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:100">
+    <row r="12" spans="1:112">
       <c r="A12" s="1">
         <v>1</v>
       </c>
@@ -4294,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:100">
+    <row r="13" spans="1:112">
       <c r="A13" s="1">
         <v>1</v>
       </c>
@@ -4596,7 +4626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:100">
+    <row r="14" spans="1:112">
       <c r="A14" s="1">
         <v>1</v>
       </c>
@@ -4679,25 +4709,25 @@
         <v>0</v>
       </c>
       <c r="AB14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14" s="1">
         <v>0</v>
@@ -4706,16 +4736,16 @@
         <v>0</v>
       </c>
       <c r="AK14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO14" s="1">
         <v>0</v>
@@ -4739,19 +4769,19 @@
         <v>0</v>
       </c>
       <c r="AV14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA14" s="1">
         <v>0</v>
@@ -4760,7 +4790,7 @@
         <v>0</v>
       </c>
       <c r="BC14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD14" s="1">
         <v>0</v>
@@ -4769,19 +4799,19 @@
         <v>0</v>
       </c>
       <c r="BF14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK14" s="1">
         <v>0</v>
@@ -4790,40 +4820,40 @@
         <v>0</v>
       </c>
       <c r="BM14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY14" s="1">
         <v>0</v>
@@ -4832,13 +4862,13 @@
         <v>0</v>
       </c>
       <c r="CA14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD14" s="1">
         <v>0</v>
@@ -4847,7 +4877,7 @@
         <v>0</v>
       </c>
       <c r="CF14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG14" s="1">
         <v>0</v>
@@ -4856,7 +4886,7 @@
         <v>0</v>
       </c>
       <c r="CI14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ14" s="1">
         <v>0</v>
@@ -4877,16 +4907,16 @@
         <v>0</v>
       </c>
       <c r="CP14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CQ14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CR14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CS14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT14" s="1">
         <v>0</v>
@@ -4897,8 +4927,20 @@
       <c r="CV14" s="1">
         <v>0</v>
       </c>
+      <c r="CW14" s="1"/>
+      <c r="CX14" s="1"/>
+      <c r="CY14" s="1"/>
+      <c r="CZ14" s="1"/>
+      <c r="DA14" s="1"/>
+      <c r="DB14" s="1"/>
+      <c r="DC14" s="1"/>
+      <c r="DD14" s="1"/>
+      <c r="DE14" s="1"/>
+      <c r="DF14" s="1"/>
+      <c r="DG14" s="1"/>
+      <c r="DH14" s="1"/>
     </row>
-    <row r="15" spans="1:100">
+    <row r="15" spans="1:112">
       <c r="A15" s="1">
         <v>1</v>
       </c>
@@ -4981,7 +5023,7 @@
         <v>0</v>
       </c>
       <c r="AB15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC15" s="1">
         <v>0</v>
@@ -4999,7 +5041,7 @@
         <v>0</v>
       </c>
       <c r="AH15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI15" s="1">
         <v>0</v>
@@ -5008,7 +5050,7 @@
         <v>0</v>
       </c>
       <c r="AK15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL15" s="1">
         <v>0</v>
@@ -5017,7 +5059,7 @@
         <v>0</v>
       </c>
       <c r="AN15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO15" s="1">
         <v>0</v>
@@ -5041,7 +5083,7 @@
         <v>0</v>
       </c>
       <c r="AV15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW15" s="1">
         <v>0</v>
@@ -5053,7 +5095,7 @@
         <v>0</v>
       </c>
       <c r="AZ15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA15" s="1">
         <v>0</v>
@@ -5062,7 +5104,7 @@
         <v>0</v>
       </c>
       <c r="BC15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD15" s="1">
         <v>0</v>
@@ -5083,7 +5125,7 @@
         <v>0</v>
       </c>
       <c r="BJ15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK15" s="1">
         <v>0</v>
@@ -5092,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="BM15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN15" s="1">
         <v>0</v>
@@ -5125,7 +5167,7 @@
         <v>0</v>
       </c>
       <c r="BX15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY15" s="1">
         <v>0</v>
@@ -5140,7 +5182,7 @@
         <v>0</v>
       </c>
       <c r="CC15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD15" s="1">
         <v>0</v>
@@ -5149,7 +5191,7 @@
         <v>0</v>
       </c>
       <c r="CF15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG15" s="1">
         <v>0</v>
@@ -5158,7 +5200,7 @@
         <v>0</v>
       </c>
       <c r="CI15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ15" s="1">
         <v>0</v>
@@ -5167,19 +5209,19 @@
         <v>0</v>
       </c>
       <c r="CL15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CQ15" s="1">
         <v>0</v>
@@ -5188,7 +5230,7 @@
         <v>0</v>
       </c>
       <c r="CS15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT15" s="1">
         <v>0</v>
@@ -5200,7 +5242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:100">
+    <row r="16" spans="1:112">
       <c r="A16" s="1">
         <v>1</v>
       </c>
@@ -5220,34 +5262,34 @@
         <v>0</v>
       </c>
       <c r="G16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="1">
         <v>0</v>
@@ -5283,7 +5325,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC16" s="1">
         <v>0</v>
@@ -5301,7 +5343,7 @@
         <v>0</v>
       </c>
       <c r="AH16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI16" s="1">
         <v>0</v>
@@ -5310,7 +5352,7 @@
         <v>0</v>
       </c>
       <c r="AK16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL16" s="1">
         <v>0</v>
@@ -5319,22 +5361,22 @@
         <v>0</v>
       </c>
       <c r="AN16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT16" s="1">
         <v>0</v>
@@ -5343,7 +5385,7 @@
         <v>0</v>
       </c>
       <c r="AV16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW16" s="1">
         <v>0</v>
@@ -5355,7 +5397,7 @@
         <v>0</v>
       </c>
       <c r="AZ16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA16" s="1">
         <v>0</v>
@@ -5364,7 +5406,7 @@
         <v>0</v>
       </c>
       <c r="BC16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD16" s="1">
         <v>0</v>
@@ -5385,7 +5427,7 @@
         <v>0</v>
       </c>
       <c r="BJ16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK16" s="1">
         <v>0</v>
@@ -5394,7 +5436,7 @@
         <v>0</v>
       </c>
       <c r="BM16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN16" s="1">
         <v>0</v>
@@ -5427,7 +5469,7 @@
         <v>0</v>
       </c>
       <c r="BX16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY16" s="1">
         <v>0</v>
@@ -5442,7 +5484,7 @@
         <v>0</v>
       </c>
       <c r="CC16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD16" s="1">
         <v>0</v>
@@ -5451,7 +5493,7 @@
         <v>0</v>
       </c>
       <c r="CF16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG16" s="1">
         <v>0</v>
@@ -5460,7 +5502,7 @@
         <v>0</v>
       </c>
       <c r="CI16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ16" s="1">
         <v>0</v>
@@ -5490,7 +5532,7 @@
         <v>0</v>
       </c>
       <c r="CS16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT16" s="1">
         <v>0</v>
@@ -5507,22 +5549,22 @@
         <v>1</v>
       </c>
       <c r="B17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" s="1">
         <v>0</v>
@@ -5531,7 +5573,7 @@
         <v>0</v>
       </c>
       <c r="J17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" s="1">
         <v>0</v>
@@ -5549,7 +5591,7 @@
         <v>0</v>
       </c>
       <c r="P17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q17" s="1">
         <v>0</v>
@@ -5558,34 +5600,34 @@
         <v>0</v>
       </c>
       <c r="S17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC17" s="1">
         <v>0</v>
@@ -5594,16 +5636,16 @@
         <v>0</v>
       </c>
       <c r="AE17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17" s="1">
         <v>0</v>
@@ -5612,7 +5654,7 @@
         <v>0</v>
       </c>
       <c r="AK17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="1">
         <v>0</v>
@@ -5621,7 +5663,7 @@
         <v>0</v>
       </c>
       <c r="AN17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO17" s="1">
         <v>0</v>
@@ -5636,7 +5678,7 @@
         <v>0</v>
       </c>
       <c r="AS17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT17" s="1">
         <v>0</v>
@@ -5645,7 +5687,7 @@
         <v>0</v>
       </c>
       <c r="AV17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW17" s="1">
         <v>0</v>
@@ -5657,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="AZ17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="1">
         <v>0</v>
@@ -5666,7 +5708,7 @@
         <v>0</v>
       </c>
       <c r="BC17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD17" s="1">
         <v>0</v>
@@ -5687,7 +5729,7 @@
         <v>0</v>
       </c>
       <c r="BJ17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK17" s="1">
         <v>0</v>
@@ -5696,22 +5738,22 @@
         <v>0</v>
       </c>
       <c r="BM17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS17" s="1">
         <v>0</v>
@@ -5729,7 +5771,7 @@
         <v>0</v>
       </c>
       <c r="BX17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY17" s="1">
         <v>0</v>
@@ -5744,7 +5786,7 @@
         <v>0</v>
       </c>
       <c r="CC17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD17" s="1">
         <v>0</v>
@@ -5753,7 +5795,7 @@
         <v>0</v>
       </c>
       <c r="CF17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG17" s="1">
         <v>0</v>
@@ -5762,7 +5804,7 @@
         <v>0</v>
       </c>
       <c r="CI17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ17" s="1">
         <v>0</v>
@@ -5792,7 +5834,7 @@
         <v>0</v>
       </c>
       <c r="CS17" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT17" s="1">
         <v>0</v>
@@ -5806,35 +5848,35 @@
     </row>
     <row r="18" spans="1:100">
       <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>0</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18" s="1">
         <v>1</v>
       </c>
-      <c r="B18" s="1">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
-        <v>0</v>
-      </c>
-      <c r="D18" s="1">
-        <v>0</v>
-      </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1">
-        <v>0</v>
-      </c>
-      <c r="I18" s="1">
-        <v>0</v>
-      </c>
-      <c r="J18" s="1">
-        <v>0</v>
-      </c>
       <c r="K18" s="1">
         <v>0</v>
       </c>
@@ -5851,7 +5893,7 @@
         <v>0</v>
       </c>
       <c r="P18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q18" s="1">
         <v>0</v>
@@ -5860,7 +5902,7 @@
         <v>0</v>
       </c>
       <c r="S18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T18" s="1">
         <v>0</v>
@@ -5896,7 +5938,7 @@
         <v>0</v>
       </c>
       <c r="AE18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF18" s="1">
         <v>0</v>
@@ -5914,7 +5956,7 @@
         <v>0</v>
       </c>
       <c r="AK18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL18" s="1">
         <v>0</v>
@@ -5923,7 +5965,7 @@
         <v>0</v>
       </c>
       <c r="AN18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO18" s="1">
         <v>0</v>
@@ -5938,7 +5980,7 @@
         <v>0</v>
       </c>
       <c r="AS18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT18" s="1">
         <v>0</v>
@@ -5947,7 +5989,7 @@
         <v>0</v>
       </c>
       <c r="AV18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW18" s="1">
         <v>0</v>
@@ -5959,7 +6001,7 @@
         <v>0</v>
       </c>
       <c r="AZ18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA18" s="1">
         <v>0</v>
@@ -5968,7 +6010,7 @@
         <v>0</v>
       </c>
       <c r="BC18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD18" s="1">
         <v>0</v>
@@ -5989,7 +6031,7 @@
         <v>0</v>
       </c>
       <c r="BJ18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK18" s="1">
         <v>0</v>
@@ -6013,7 +6055,7 @@
         <v>0</v>
       </c>
       <c r="BR18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS18" s="1">
         <v>0</v>
@@ -6031,7 +6073,7 @@
         <v>0</v>
       </c>
       <c r="BX18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY18" s="1">
         <v>0</v>
@@ -6046,7 +6088,7 @@
         <v>0</v>
       </c>
       <c r="CC18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD18" s="1">
         <v>0</v>
@@ -6055,7 +6097,7 @@
         <v>0</v>
       </c>
       <c r="CF18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG18" s="1">
         <v>0</v>
@@ -6064,16 +6106,16 @@
         <v>0</v>
       </c>
       <c r="CI18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CK18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CL18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM18" s="1">
         <v>0</v>
@@ -6094,7 +6136,7 @@
         <v>0</v>
       </c>
       <c r="CS18" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT18" s="1">
         <v>0</v>
@@ -6108,43 +6150,43 @@
     </row>
     <row r="19" spans="1:100">
       <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1">
+        <v>0</v>
+      </c>
+      <c r="C19" s="1">
+        <v>0</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1">
+        <v>0</v>
+      </c>
+      <c r="I19" s="1">
+        <v>0</v>
+      </c>
+      <c r="J19" s="1">
         <v>1</v>
       </c>
-      <c r="B19" s="1">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0</v>
-      </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="F19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>0</v>
-      </c>
-      <c r="I19" s="1">
-        <v>0</v>
-      </c>
-      <c r="J19" s="1">
-        <v>0</v>
-      </c>
       <c r="K19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="1">
         <v>0</v>
@@ -6153,7 +6195,7 @@
         <v>0</v>
       </c>
       <c r="P19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="1">
         <v>0</v>
@@ -6162,7 +6204,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="1">
         <v>0</v>
@@ -6198,7 +6240,7 @@
         <v>0</v>
       </c>
       <c r="AE19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF19" s="1">
         <v>0</v>
@@ -6213,10 +6255,10 @@
         <v>0</v>
       </c>
       <c r="AJ19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL19" s="1">
         <v>0</v>
@@ -6225,7 +6267,7 @@
         <v>0</v>
       </c>
       <c r="AN19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO19" s="1">
         <v>0</v>
@@ -6240,7 +6282,7 @@
         <v>0</v>
       </c>
       <c r="AS19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT19" s="1">
         <v>0</v>
@@ -6249,10 +6291,10 @@
         <v>0</v>
       </c>
       <c r="AV19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX19" s="1">
         <v>0</v>
@@ -6261,7 +6303,7 @@
         <v>0</v>
       </c>
       <c r="AZ19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA19" s="1">
         <v>0</v>
@@ -6270,7 +6312,7 @@
         <v>0</v>
       </c>
       <c r="BC19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD19" s="1">
         <v>0</v>
@@ -6279,19 +6321,19 @@
         <v>0</v>
       </c>
       <c r="BF19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK19" s="1">
         <v>0</v>
@@ -6315,7 +6357,7 @@
         <v>0</v>
       </c>
       <c r="BR19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS19" s="1">
         <v>0</v>
@@ -6333,31 +6375,31 @@
         <v>0</v>
       </c>
       <c r="BX19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG19" s="1">
         <v>0</v>
@@ -6366,7 +6408,7 @@
         <v>0</v>
       </c>
       <c r="CI19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ19" s="1">
         <v>0</v>
@@ -6375,7 +6417,7 @@
         <v>0</v>
       </c>
       <c r="CL19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM19" s="1">
         <v>0</v>
@@ -6384,19 +6426,19 @@
         <v>0</v>
       </c>
       <c r="CO19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CQ19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CR19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CS19" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT19" s="1">
         <v>0</v>
@@ -6410,34 +6452,34 @@
     </row>
     <row r="20" spans="1:100">
       <c r="A20" s="1">
+        <v>0</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0</v>
+      </c>
+      <c r="E20" s="1">
         <v>1</v>
       </c>
-      <c r="B20" s="1">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
-        <v>0</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0</v>
-      </c>
-      <c r="E20" s="1">
-        <v>0</v>
-      </c>
       <c r="F20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="1">
         <v>0</v>
@@ -6446,7 +6488,7 @@
         <v>0</v>
       </c>
       <c r="M20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N20" s="1">
         <v>0</v>
@@ -6455,7 +6497,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="1">
         <v>0</v>
@@ -6464,34 +6506,34 @@
         <v>0</v>
       </c>
       <c r="S20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC20" s="1">
         <v>0</v>
@@ -6500,22 +6542,22 @@
         <v>0</v>
       </c>
       <c r="AE20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK20" s="1">
         <v>0</v>
@@ -6527,7 +6569,7 @@
         <v>0</v>
       </c>
       <c r="AN20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO20" s="1">
         <v>0</v>
@@ -6542,7 +6584,7 @@
         <v>0</v>
       </c>
       <c r="AS20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT20" s="1">
         <v>0</v>
@@ -6554,7 +6596,7 @@
         <v>0</v>
       </c>
       <c r="AW20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX20" s="1">
         <v>0</v>
@@ -6563,7 +6605,7 @@
         <v>0</v>
       </c>
       <c r="AZ20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA20" s="1">
         <v>0</v>
@@ -6572,7 +6614,7 @@
         <v>0</v>
       </c>
       <c r="BC20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD20" s="1">
         <v>0</v>
@@ -6581,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="BF20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG20" s="1">
         <v>0</v>
@@ -6602,22 +6644,22 @@
         <v>0</v>
       </c>
       <c r="BM20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS20" s="1">
         <v>0</v>
@@ -6650,7 +6692,7 @@
         <v>0</v>
       </c>
       <c r="CC20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD20" s="1">
         <v>0</v>
@@ -6668,7 +6710,7 @@
         <v>0</v>
       </c>
       <c r="CI20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ20" s="1">
         <v>0</v>
@@ -6677,7 +6719,7 @@
         <v>0</v>
       </c>
       <c r="CL20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM20" s="1">
         <v>0</v>
@@ -6686,7 +6728,7 @@
         <v>0</v>
       </c>
       <c r="CO20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP20" s="1">
         <v>0</v>
@@ -6698,7 +6740,7 @@
         <v>0</v>
       </c>
       <c r="CS20" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT20" s="1">
         <v>0</v>
@@ -6712,20 +6754,20 @@
     </row>
     <row r="21" spans="1:100">
       <c r="A21" s="1">
+        <v>0</v>
+      </c>
+      <c r="B21" s="1">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
         <v>1</v>
       </c>
-      <c r="B21" s="1">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
-        <v>0</v>
-      </c>
-      <c r="D21" s="1">
-        <v>0</v>
-      </c>
-      <c r="E21" s="1">
-        <v>0</v>
-      </c>
       <c r="F21" s="1">
         <v>0</v>
       </c>
@@ -6748,7 +6790,7 @@
         <v>0</v>
       </c>
       <c r="M21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N21" s="1">
         <v>0</v>
@@ -6757,7 +6799,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="1">
         <v>0</v>
@@ -6793,7 +6835,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21" s="1">
         <v>0</v>
@@ -6814,7 +6856,7 @@
         <v>0</v>
       </c>
       <c r="AI21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ21" s="1">
         <v>0</v>
@@ -6829,7 +6871,7 @@
         <v>0</v>
       </c>
       <c r="AN21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO21" s="1">
         <v>0</v>
@@ -6844,7 +6886,7 @@
         <v>0</v>
       </c>
       <c r="AS21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT21" s="1">
         <v>0</v>
@@ -6856,7 +6898,7 @@
         <v>0</v>
       </c>
       <c r="AW21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX21" s="1">
         <v>0</v>
@@ -6865,7 +6907,7 @@
         <v>0</v>
       </c>
       <c r="AZ21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA21" s="1">
         <v>0</v>
@@ -6874,7 +6916,7 @@
         <v>0</v>
       </c>
       <c r="BC21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD21" s="1">
         <v>0</v>
@@ -6883,7 +6925,7 @@
         <v>0</v>
       </c>
       <c r="BF21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG21" s="1">
         <v>0</v>
@@ -6904,7 +6946,7 @@
         <v>0</v>
       </c>
       <c r="BM21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN21" s="1">
         <v>0</v>
@@ -6952,7 +6994,7 @@
         <v>0</v>
       </c>
       <c r="CC21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD21" s="1">
         <v>0</v>
@@ -6970,7 +7012,7 @@
         <v>0</v>
       </c>
       <c r="CI21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ21" s="1">
         <v>0</v>
@@ -6979,7 +7021,7 @@
         <v>0</v>
       </c>
       <c r="CL21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM21" s="1">
         <v>0</v>
@@ -6988,7 +7030,7 @@
         <v>0</v>
       </c>
       <c r="CO21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP21" s="1">
         <v>0</v>
@@ -7000,7 +7042,7 @@
         <v>0</v>
       </c>
       <c r="CS21" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT21" s="1">
         <v>0</v>
@@ -7014,20 +7056,20 @@
     </row>
     <row r="22" spans="1:100">
       <c r="A22" s="1">
+        <v>0</v>
+      </c>
+      <c r="B22" s="1">
+        <v>0</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="1">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
-        <v>0</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
       <c r="F22" s="1">
         <v>0</v>
       </c>
@@ -7050,7 +7092,7 @@
         <v>0</v>
       </c>
       <c r="M22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="1">
         <v>0</v>
@@ -7059,7 +7101,7 @@
         <v>0</v>
       </c>
       <c r="P22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="1">
         <v>0</v>
@@ -7095,7 +7137,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC22" s="1">
         <v>0</v>
@@ -7116,7 +7158,7 @@
         <v>0</v>
       </c>
       <c r="AI22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ22" s="1">
         <v>0</v>
@@ -7131,7 +7173,7 @@
         <v>0</v>
       </c>
       <c r="AN22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO22" s="1">
         <v>0</v>
@@ -7146,19 +7188,19 @@
         <v>0</v>
       </c>
       <c r="AS22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX22" s="1">
         <v>0</v>
@@ -7167,7 +7209,7 @@
         <v>0</v>
       </c>
       <c r="AZ22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA22" s="1">
         <v>0</v>
@@ -7176,7 +7218,7 @@
         <v>0</v>
       </c>
       <c r="BC22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD22" s="1">
         <v>0</v>
@@ -7185,7 +7227,7 @@
         <v>0</v>
       </c>
       <c r="BF22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG22" s="1">
         <v>0</v>
@@ -7206,7 +7248,7 @@
         <v>0</v>
       </c>
       <c r="BM22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN22" s="1">
         <v>0</v>
@@ -7254,7 +7296,7 @@
         <v>0</v>
       </c>
       <c r="CC22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD22" s="1">
         <v>0</v>
@@ -7272,7 +7314,7 @@
         <v>0</v>
       </c>
       <c r="CI22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ22" s="1">
         <v>0</v>
@@ -7281,16 +7323,16 @@
         <v>0</v>
       </c>
       <c r="CL22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CM22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CN22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CO22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP22" s="1">
         <v>0</v>
@@ -7302,7 +7344,7 @@
         <v>0</v>
       </c>
       <c r="CS22" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT22" s="1">
         <v>0</v>
@@ -7325,10 +7367,10 @@
         <v>0</v>
       </c>
       <c r="D23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F23" s="1">
         <v>0</v>
@@ -7337,22 +7379,22 @@
         <v>0</v>
       </c>
       <c r="H23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="1">
         <v>0</v>
@@ -7361,43 +7403,43 @@
         <v>0</v>
       </c>
       <c r="P23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC23" s="1">
         <v>0</v>
@@ -7418,22 +7460,22 @@
         <v>0</v>
       </c>
       <c r="AI23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO23" s="1">
         <v>0</v>
@@ -7442,13 +7484,13 @@
         <v>0</v>
       </c>
       <c r="AQ23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT23" s="1">
         <v>0</v>
@@ -7469,61 +7511,61 @@
         <v>0</v>
       </c>
       <c r="AZ23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS23" s="1">
         <v>0</v>
@@ -7556,25 +7598,25 @@
         <v>0</v>
       </c>
       <c r="CC23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CF23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CG23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CH23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CI23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CJ23" s="1">
         <v>0</v>
@@ -7592,10 +7634,10 @@
         <v>0</v>
       </c>
       <c r="CO23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CP23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CQ23" s="1">
         <v>0</v>
@@ -7604,323 +7646,323 @@
         <v>0</v>
       </c>
       <c r="CS23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CT23" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CU23" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="CV23" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:100">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1">
-        <v>0</v>
-      </c>
-      <c r="C24" s="1">
-        <v>0</v>
-      </c>
-      <c r="D24" s="1">
-        <v>0</v>
-      </c>
-      <c r="E24" s="1">
-        <v>0</v>
-      </c>
-      <c r="F24" s="1">
-        <v>0</v>
-      </c>
-      <c r="G24" s="1">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1">
-        <v>0</v>
-      </c>
-      <c r="I24" s="1">
-        <v>0</v>
-      </c>
-      <c r="J24" s="1">
-        <v>0</v>
-      </c>
-      <c r="K24" s="1">
-        <v>0</v>
-      </c>
-      <c r="L24" s="1">
-        <v>0</v>
-      </c>
-      <c r="M24" s="1">
-        <v>0</v>
-      </c>
-      <c r="N24" s="1">
-        <v>0</v>
-      </c>
-      <c r="O24" s="1">
-        <v>0</v>
-      </c>
-      <c r="P24" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q24" s="1">
-        <v>0</v>
-      </c>
-      <c r="R24" s="1">
-        <v>0</v>
-      </c>
-      <c r="S24" s="1">
-        <v>0</v>
-      </c>
-      <c r="T24" s="1">
-        <v>0</v>
-      </c>
-      <c r="U24" s="1">
-        <v>0</v>
-      </c>
-      <c r="V24" s="1">
-        <v>0</v>
-      </c>
-      <c r="W24" s="1">
-        <v>0</v>
-      </c>
-      <c r="X24" s="1">
-        <v>0</v>
-      </c>
-      <c r="Y24" s="1">
-        <v>0</v>
-      </c>
-      <c r="Z24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AA24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AB24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AC24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AD24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AE24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AF24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AG24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AH24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AI24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AJ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AK24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AL24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AM24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AN24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AO24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AP24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AQ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AR24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AS24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AT24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AU24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AV24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AW24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AX24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AY24" s="1">
-        <v>0</v>
-      </c>
-      <c r="AZ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BA24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BB24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BC24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BD24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BF24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BG24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BJ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BK24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BL24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BM24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BN24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BO24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BP24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BQ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BR24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BS24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BT24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BU24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BV24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BW24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BX24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BY24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BZ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CA24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CB24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CC24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CD24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CE24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CF24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CG24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CH24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CI24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CJ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CK24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CL24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CM24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CN24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CO24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CP24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CQ24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CR24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CS24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CT24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CU24" s="1">
-        <v>0</v>
-      </c>
-      <c r="CV24" s="1">
+      <c r="A24" s="4">
+        <v>0</v>
+      </c>
+      <c r="B24" s="4">
+        <v>0</v>
+      </c>
+      <c r="C24" s="4">
+        <v>0</v>
+      </c>
+      <c r="D24" s="4">
+        <v>0</v>
+      </c>
+      <c r="E24" s="4">
+        <v>0</v>
+      </c>
+      <c r="F24" s="4">
+        <v>0</v>
+      </c>
+      <c r="G24" s="4">
+        <v>0</v>
+      </c>
+      <c r="H24" s="4">
+        <v>0</v>
+      </c>
+      <c r="I24" s="4">
+        <v>0</v>
+      </c>
+      <c r="J24" s="4">
+        <v>0</v>
+      </c>
+      <c r="K24" s="4">
+        <v>0</v>
+      </c>
+      <c r="L24" s="4">
+        <v>0</v>
+      </c>
+      <c r="M24" s="4">
+        <v>0</v>
+      </c>
+      <c r="N24" s="4">
+        <v>0</v>
+      </c>
+      <c r="O24" s="4">
+        <v>0</v>
+      </c>
+      <c r="P24" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="4">
+        <v>0</v>
+      </c>
+      <c r="R24" s="4">
+        <v>0</v>
+      </c>
+      <c r="S24" s="4">
+        <v>0</v>
+      </c>
+      <c r="T24" s="4">
+        <v>0</v>
+      </c>
+      <c r="U24" s="4">
+        <v>0</v>
+      </c>
+      <c r="V24" s="4">
+        <v>0</v>
+      </c>
+      <c r="W24" s="4">
+        <v>0</v>
+      </c>
+      <c r="X24" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y24" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY24" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BB24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BF24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BH24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BI24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BJ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BK24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BL24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BM24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BN24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BO24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BP24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BQ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BR24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BS24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BT24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BU24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BV24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BW24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BX24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BY24" s="4">
+        <v>0</v>
+      </c>
+      <c r="BZ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CA24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CB24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CC24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CD24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CE24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CF24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CG24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CH24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CI24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CJ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CK24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CL24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CM24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CN24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CO24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CP24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CQ24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CR24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CS24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CT24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CU24" s="4">
+        <v>0</v>
+      </c>
+      <c r="CV24" s="4">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:100">
       <c r="A25" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -8222,7 +8264,7 @@
     </row>
     <row r="26" spans="1:100">
       <c r="A26" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B26" s="1">
         <v>0</v>
@@ -8524,7 +8566,7 @@
     </row>
     <row r="27" spans="1:100">
       <c r="A27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B27" s="1">
         <v>0</v>
@@ -8826,7 +8868,7 @@
     </row>
     <row r="28" spans="1:100">
       <c r="A28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B28" s="1">
         <v>0</v>
@@ -9128,7 +9170,7 @@
     </row>
     <row r="29" spans="1:100">
       <c r="A29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -9430,7 +9472,7 @@
     </row>
     <row r="30" spans="1:100">
       <c r="A30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -9732,7 +9774,7 @@
     </row>
     <row r="31" spans="1:100">
       <c r="A31" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -10034,7 +10076,7 @@
     </row>
     <row r="32" spans="1:100">
       <c r="A32" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -10336,7 +10378,7 @@
     </row>
     <row r="33" spans="1:100">
       <c r="A33" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -10638,28 +10680,28 @@
     </row>
     <row r="34" spans="1:100">
       <c r="A34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H34" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I34" s="1">
         <v>0</v>
@@ -10961,7 +11003,7 @@
         <v>0</v>
       </c>
       <c r="H35" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I35" s="1">
         <v>0</v>
@@ -11263,7 +11305,7 @@
         <v>0</v>
       </c>
       <c r="H36" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I36" s="1">
         <v>0</v>
@@ -11565,7 +11607,7 @@
         <v>0</v>
       </c>
       <c r="H37" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I37" s="1">
         <v>0</v>
@@ -11867,7 +11909,7 @@
         <v>0</v>
       </c>
       <c r="H38" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I38" s="1">
         <v>0</v>
@@ -12169,7 +12211,7 @@
         <v>0</v>
       </c>
       <c r="H39" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I39" s="1">
         <v>0</v>
@@ -12471,7 +12513,7 @@
         <v>0</v>
       </c>
       <c r="H40" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" s="1">
         <v>0</v>
@@ -12773,7 +12815,7 @@
         <v>0</v>
       </c>
       <c r="H41" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I41" s="1">
         <v>0</v>
@@ -13075,7 +13117,7 @@
         <v>0</v>
       </c>
       <c r="H42" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" s="1">
         <v>0</v>
@@ -13377,7 +13419,7 @@
         <v>0</v>
       </c>
       <c r="H43" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I43" s="1">
         <v>0</v>
@@ -13679,7 +13721,7 @@
         <v>0</v>
       </c>
       <c r="H44" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I44" s="1">
         <v>0</v>
@@ -13981,7 +14023,7 @@
         <v>0</v>
       </c>
       <c r="H45" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I45" s="1">
         <v>0</v>
@@ -14283,7 +14325,7 @@
         <v>0</v>
       </c>
       <c r="H46" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I46" s="1">
         <v>0</v>
@@ -14585,7 +14627,7 @@
         <v>0</v>
       </c>
       <c r="H47" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I47" s="1">
         <v>0</v>
@@ -14887,7 +14929,7 @@
         <v>0</v>
       </c>
       <c r="H48" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I48" s="1">
         <v>0</v>
@@ -15189,7 +15231,7 @@
         <v>0</v>
       </c>
       <c r="H49" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="1">
         <v>0</v>
@@ -15491,7 +15533,7 @@
         <v>0</v>
       </c>
       <c r="H50" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I50" s="1">
         <v>0</v>
@@ -15793,7 +15835,7 @@
         <v>0</v>
       </c>
       <c r="H51" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I51" s="1">
         <v>0</v>
@@ -16095,7 +16137,7 @@
         <v>0</v>
       </c>
       <c r="H52" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I52" s="1">
         <v>0</v>
@@ -16397,7 +16439,7 @@
         <v>0</v>
       </c>
       <c r="H53" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I53" s="1">
         <v>0</v>
@@ -16699,7 +16741,7 @@
         <v>0</v>
       </c>
       <c r="H54" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I54" s="1">
         <v>0</v>
@@ -17001,7 +17043,7 @@
         <v>0</v>
       </c>
       <c r="H55" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I55" s="1">
         <v>0</v>
@@ -17303,7 +17345,7 @@
         <v>0</v>
       </c>
       <c r="H56" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I56" s="1">
         <v>0</v>
@@ -17605,7 +17647,7 @@
         <v>0</v>
       </c>
       <c r="H57" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I57" s="1">
         <v>0</v>
@@ -17907,7 +17949,7 @@
         <v>0</v>
       </c>
       <c r="H58" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I58" s="1">
         <v>0</v>
@@ -18209,7 +18251,7 @@
         <v>0</v>
       </c>
       <c r="H59" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I59" s="1">
         <v>0</v>
@@ -18511,7 +18553,7 @@
         <v>0</v>
       </c>
       <c r="H60" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I60" s="1">
         <v>0</v>
@@ -18813,7 +18855,7 @@
         <v>0</v>
       </c>
       <c r="H61" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I61" s="1">
         <v>0</v>
@@ -19115,7 +19157,7 @@
         <v>0</v>
       </c>
       <c r="H62" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I62" s="1">
         <v>0</v>
@@ -19417,7 +19459,7 @@
         <v>0</v>
       </c>
       <c r="H63" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I63" s="1">
         <v>0</v>
@@ -19719,7 +19761,7 @@
         <v>0</v>
       </c>
       <c r="H64" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" s="1">
         <v>0</v>
@@ -20021,7 +20063,7 @@
         <v>0</v>
       </c>
       <c r="H65" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" s="1">
         <v>0</v>
@@ -20323,7 +20365,7 @@
         <v>0</v>
       </c>
       <c r="H66" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I66" s="1">
         <v>0</v>
@@ -20625,7 +20667,7 @@
         <v>0</v>
       </c>
       <c r="H67" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I67" s="1">
         <v>0</v>
@@ -20927,7 +20969,7 @@
         <v>0</v>
       </c>
       <c r="H68" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I68" s="1">
         <v>0</v>
@@ -21229,7 +21271,7 @@
         <v>0</v>
       </c>
       <c r="H69" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I69" s="1">
         <v>0</v>
@@ -21531,7 +21573,7 @@
         <v>0</v>
       </c>
       <c r="H70" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I70" s="1">
         <v>0</v>
@@ -21833,7 +21875,7 @@
         <v>0</v>
       </c>
       <c r="H71" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I71" s="1">
         <v>0</v>
@@ -22135,7 +22177,7 @@
         <v>0</v>
       </c>
       <c r="H72" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I72" s="1">
         <v>0</v>
@@ -22437,7 +22479,7 @@
         <v>0</v>
       </c>
       <c r="H73" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I73" s="1">
         <v>0</v>
@@ -22724,22 +22766,22 @@
         <v>0</v>
       </c>
       <c r="C74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H74" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I74" s="1">
         <v>0</v>
@@ -23026,7 +23068,7 @@
         <v>0</v>
       </c>
       <c r="C75" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D75" s="1">
         <v>0</v>
@@ -23328,7 +23370,7 @@
         <v>0</v>
       </c>
       <c r="C76" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D76" s="1">
         <v>0</v>
@@ -23630,7 +23672,7 @@
         <v>0</v>
       </c>
       <c r="C77" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D77" s="1">
         <v>0</v>
@@ -23932,7 +23974,7 @@
         <v>0</v>
       </c>
       <c r="C78" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D78" s="1">
         <v>0</v>
@@ -24234,7 +24276,7 @@
         <v>0</v>
       </c>
       <c r="C79" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D79" s="1">
         <v>0</v>
@@ -24536,7 +24578,7 @@
         <v>0</v>
       </c>
       <c r="C80" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" s="1">
         <v>0</v>
@@ -24838,7 +24880,7 @@
         <v>0</v>
       </c>
       <c r="C81" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" s="1">
         <v>0</v>
@@ -25140,7 +25182,7 @@
         <v>0</v>
       </c>
       <c r="C82" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" s="1">
         <v>0</v>
@@ -25442,7 +25484,7 @@
         <v>0</v>
       </c>
       <c r="C83" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D83" s="1">
         <v>0</v>
@@ -25744,7 +25786,7 @@
         <v>0</v>
       </c>
       <c r="C84" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D84" s="1">
         <v>0</v>
@@ -26046,7 +26088,7 @@
         <v>0</v>
       </c>
       <c r="C85" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D85" s="1">
         <v>0</v>
@@ -26348,7 +26390,7 @@
         <v>0</v>
       </c>
       <c r="C86" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D86" s="1">
         <v>0</v>
@@ -26650,7 +26692,7 @@
         <v>0</v>
       </c>
       <c r="C87" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D87" s="1">
         <v>0</v>
@@ -26952,7 +26994,7 @@
         <v>0</v>
       </c>
       <c r="C88" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D88" s="1">
         <v>0</v>
@@ -27254,7 +27296,7 @@
         <v>0</v>
       </c>
       <c r="C89" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D89" s="1">
         <v>0</v>
@@ -27556,7 +27598,7 @@
         <v>0</v>
       </c>
       <c r="C90" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D90" s="1">
         <v>0</v>
@@ -27858,7 +27900,7 @@
         <v>0</v>
       </c>
       <c r="C91" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D91" s="1">
         <v>0</v>
@@ -28160,7 +28202,7 @@
         <v>0</v>
       </c>
       <c r="C92" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D92" s="1">
         <v>0</v>
@@ -28462,7 +28504,7 @@
         <v>0</v>
       </c>
       <c r="C93" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D93" s="1">
         <v>0</v>
@@ -28764,7 +28806,7 @@
         <v>0</v>
       </c>
       <c r="C94" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D94" s="1">
         <v>0</v>
@@ -29066,7 +29108,7 @@
         <v>0</v>
       </c>
       <c r="C95" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D95" s="1">
         <v>0</v>
@@ -29368,7 +29410,7 @@
         <v>0</v>
       </c>
       <c r="C96" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D96" s="1">
         <v>0</v>
@@ -29670,7 +29712,7 @@
         <v>0</v>
       </c>
       <c r="C97" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D97" s="1">
         <v>0</v>
@@ -29972,7 +30014,7 @@
         <v>0</v>
       </c>
       <c r="C98" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D98" s="1">
         <v>0</v>
@@ -30274,7 +30316,7 @@
         <v>0</v>
       </c>
       <c r="C99" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D99" s="1">
         <v>0</v>
@@ -30576,7 +30618,7 @@
         <v>0</v>
       </c>
       <c r="C100" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D100" s="1">
         <v>0</v>
@@ -30878,7 +30920,7 @@
         <v>0</v>
       </c>
       <c r="C101" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D101" s="1">
         <v>0</v>
@@ -31180,7 +31222,7 @@
         <v>0</v>
       </c>
       <c r="C102" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D102" s="1">
         <v>0</v>
@@ -31482,7 +31524,7 @@
         <v>0</v>
       </c>
       <c r="C103" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D103" s="1">
         <v>0</v>
@@ -31784,7 +31826,7 @@
         <v>0</v>
       </c>
       <c r="C104" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D104" s="1">
         <v>0</v>
@@ -32086,7 +32128,7 @@
         <v>0</v>
       </c>
       <c r="C105" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D105" s="1">
         <v>0</v>
@@ -32388,7 +32430,7 @@
         <v>0</v>
       </c>
       <c r="C106" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D106" s="1">
         <v>0</v>
@@ -32690,7 +32732,7 @@
         <v>0</v>
       </c>
       <c r="C107" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D107" s="1">
         <v>0</v>
@@ -32992,7 +33034,7 @@
         <v>0</v>
       </c>
       <c r="C108" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D108" s="1">
         <v>0</v>
@@ -33294,40 +33336,40 @@
         <v>0</v>
       </c>
       <c r="C109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N109" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O109" s="1">
         <v>0</v>
@@ -33629,7 +33671,7 @@
         <v>0</v>
       </c>
       <c r="N110" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O110" s="1">
         <v>0</v>
@@ -33931,7 +33973,7 @@
         <v>0</v>
       </c>
       <c r="N111" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O111" s="1">
         <v>0</v>
@@ -34233,7 +34275,7 @@
         <v>0</v>
       </c>
       <c r="N112" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O112" s="1">
         <v>0</v>
@@ -34535,37 +34577,37 @@
         <v>0</v>
       </c>
       <c r="N113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V113" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W113" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="X113" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y113" s="1">
         <v>0</v>
@@ -36609,7 +36651,127 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A14:CQ28 A112:CQ113">
+  <conditionalFormatting sqref="A112:A113 A14 C16:D25 AZ16:CQ28 Y16:Y25 AC112:CQ113 B15:CQ15">
+    <cfRule type="colorScale" priority="35">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A13">
+    <cfRule type="colorScale" priority="34">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CR15:CV28 CR112:CV113 CW14:DH14">
+    <cfRule type="colorScale" priority="33">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A98:A111 AC98:CQ111">
+    <cfRule type="colorScale" priority="32">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CR98:CV111">
+    <cfRule type="colorScale" priority="31">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A57:A65 A93:A97 AC93:CQ97 AC57:CQ65">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CR57:CV65 CR93:CV97">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A43:A56 AC43:CQ56">
+    <cfRule type="colorScale" priority="28">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CR43:CV56">
+    <cfRule type="colorScale" priority="27">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AZ29:CQ31 A42 AC32:CQ42">
+    <cfRule type="colorScale" priority="26">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CR29:CV42">
+    <cfRule type="colorScale" priority="25">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A89:A92 AC89:CQ92">
+    <cfRule type="colorScale" priority="24">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="CR89:CV92">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36619,7 +36781,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:A13">
+  <conditionalFormatting sqref="A84:A88 AC84:CQ88">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36629,7 +36791,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR14:CV28 CR112:CV113">
+  <conditionalFormatting sqref="CR84:CV88">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36639,7 +36801,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A98:CQ111">
+  <conditionalFormatting sqref="A80:A83 AC80:CQ83">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36649,7 +36811,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR98:CV111">
+  <conditionalFormatting sqref="CR80:CV83">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36659,7 +36821,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A57:CQ65 A93:CQ97">
+  <conditionalFormatting sqref="A75:A79 AC75:CQ79">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36669,7 +36831,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR57:CV65 CR93:CV97">
+  <conditionalFormatting sqref="CR75:CV79">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36679,7 +36841,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A43:CQ56">
+  <conditionalFormatting sqref="A71:A74 AC71:CQ74">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36689,7 +36851,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR43:CV56">
+  <conditionalFormatting sqref="CR71:CV74">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36699,7 +36861,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A29:CQ42">
+  <conditionalFormatting sqref="A66:A70 AC66:CQ70">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36709,7 +36871,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR29:CV42">
+  <conditionalFormatting sqref="CR66:CV70">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36719,67 +36881,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A89:CQ92">
-    <cfRule type="colorScale" priority="12">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CR89:CV92">
-    <cfRule type="colorScale" priority="11">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A84:CQ88">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CR84:CV88">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A80:CQ83">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="CR80:CV83">
-    <cfRule type="colorScale" priority="7">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A75:CQ79">
+  <conditionalFormatting sqref="Z16:AY25 AC26:AY31">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36789,7 +36891,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR75:CV79">
+  <conditionalFormatting sqref="E16:X25">
     <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36799,7 +36901,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A71:CQ74">
+  <conditionalFormatting sqref="A16:B25 A26:A41">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36809,7 +36911,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR71:CV74">
+  <conditionalFormatting sqref="B26:AB113">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36819,7 +36921,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A66:CQ70">
+  <conditionalFormatting sqref="A15">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -36829,7 +36931,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR66:CV70">
+  <conditionalFormatting sqref="B14:CV14">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Test #10. Full puzzle size with first cut at puzzle. Tried to reduce bump more, but my calculations seem off, so I'll have to look at this again next time. Next, try to put puzzle in lid...
The diameter of this puzzle is very close (almost identical) to the full size puzzle from Thingiverse.
But the height is too short.  The thingiverse puzzle is 106mm tall.  So I can increase the size of
this puzzle quite a bit.  (its currently approximately 80mm tall).
</commit_message>
<xml_diff>
--- a/Labyrinth_maze.xlsx
+++ b/Labyrinth_maze.xlsx
@@ -74,8 +74,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="111">
+  <cellStyleXfs count="113">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -200,7 +202,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="111">
+  <cellStyles count="113">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -256,6 +258,7 @@
     <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -311,6 +314,7 @@
     <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -642,14 +646,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DH122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="65" zoomScaleNormal="65" zoomScalePageLayoutView="65" workbookViewId="0">
-      <selection activeCell="AH13" sqref="AH13"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="AK10" sqref="AK10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="19" width="6.5" style="1" customWidth="1"/>
-    <col min="20" max="100" width="6.5" customWidth="1"/>
+    <col min="1" max="19" width="4.33203125" style="1" customWidth="1"/>
+    <col min="20" max="41" width="4.33203125" customWidth="1"/>
+    <col min="42" max="100" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:112">
@@ -1918,10 +1923,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1936,7 +1941,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" s="2">
         <v>1</v>
@@ -1951,10 +1956,10 @@
         <v>1</v>
       </c>
       <c r="M7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O7" s="2">
         <v>1</v>
@@ -1978,28 +1983,28 @@
         <v>1</v>
       </c>
       <c r="V7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X7" s="2">
         <v>1</v>
       </c>
       <c r="Y7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD7" s="2">
         <v>0</v>
@@ -2014,19 +2019,19 @@
         <v>0</v>
       </c>
       <c r="AH7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM7" s="2">
         <v>0</v>
@@ -2117,13 +2122,13 @@
     </row>
     <row r="8" spans="1:112">
       <c r="A8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2">
         <v>0</v>
@@ -2138,10 +2143,10 @@
         <v>0</v>
       </c>
       <c r="H8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8" s="2">
         <v>0</v>
@@ -2177,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="U8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V8" s="2">
         <v>0</v>
@@ -2201,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="AC8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD8" s="2">
         <v>0</v>
@@ -2216,7 +2221,7 @@
         <v>0</v>
       </c>
       <c r="AH8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="2">
         <v>0</v>
@@ -2225,10 +2230,10 @@
         <v>0</v>
       </c>
       <c r="AK8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM8" s="2">
         <v>0</v>
@@ -2319,31 +2324,31 @@
     </row>
     <row r="9" spans="1:112">
       <c r="A9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="2">
         <v>1</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="2">
         <v>1</v>
       </c>
       <c r="I9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J9" s="2">
         <v>0</v>
@@ -2379,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="U9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V9" s="2">
         <v>0</v>
@@ -2397,19 +2402,19 @@
         <v>0</v>
       </c>
       <c r="AA9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC9" s="2">
         <v>1</v>
       </c>
       <c r="AD9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AE9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF9" s="2">
         <v>0</v>
@@ -2418,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="AH9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI9" s="2">
         <v>0</v>
@@ -2427,10 +2432,10 @@
         <v>0</v>
       </c>
       <c r="AK9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM9" s="2">
         <v>0</v>
@@ -2527,13 +2532,13 @@
         <v>0</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2">
         <v>0</v>
       </c>
       <c r="E10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F10" s="2">
         <v>0</v>
@@ -2542,7 +2547,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I10" s="2">
         <v>0</v>
@@ -2581,58 +2586,58 @@
         <v>0</v>
       </c>
       <c r="U10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10" s="2">
         <v>0</v>
       </c>
       <c r="AC10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE10" s="2">
         <v>1</v>
       </c>
       <c r="AF10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK10" s="2">
         <v>1</v>
       </c>
       <c r="AL10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM10" s="2">
         <v>0</v>
@@ -2729,13 +2734,13 @@
         <v>0</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2">
         <v>0</v>
       </c>
       <c r="E11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="2">
         <v>0</v>
@@ -2744,7 +2749,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -2768,10 +2773,10 @@
         <v>1</v>
       </c>
       <c r="P11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R11" s="2">
         <v>1</v>
@@ -2783,7 +2788,7 @@
         <v>0</v>
       </c>
       <c r="U11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="2">
         <v>0</v>
@@ -2807,13 +2812,13 @@
         <v>0</v>
       </c>
       <c r="AC11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD11" s="2">
         <v>0</v>
       </c>
       <c r="AE11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF11" s="2">
         <v>0</v>
@@ -2825,16 +2830,16 @@
         <v>0</v>
       </c>
       <c r="AI11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11" s="2">
         <v>0</v>
       </c>
       <c r="AK11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM11" s="2">
         <v>0</v>
@@ -2925,16 +2930,16 @@
     </row>
     <row r="12" spans="1:112">
       <c r="A12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B12" s="2">
         <v>0</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2">
         <v>1</v>
@@ -2949,73 +2954,73 @@
         <v>1</v>
       </c>
       <c r="I12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L12" s="2">
         <v>1</v>
       </c>
       <c r="M12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U12" s="2">
         <v>1</v>
       </c>
       <c r="V12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD12" s="2">
         <v>0</v>
       </c>
       <c r="AE12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF12" s="2">
         <v>0</v>
@@ -3027,22 +3032,22 @@
         <v>0</v>
       </c>
       <c r="AI12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ12" s="2">
         <v>0</v>
       </c>
       <c r="AK12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL12" s="2">
         <v>1</v>
       </c>
       <c r="AM12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN12" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AO12" s="4">
         <v>0</v>
@@ -3126,124 +3131,124 @@
       <c r="CV12" s="2"/>
     </row>
     <row r="13" spans="1:112">
-      <c r="A13" s="4">
-        <v>0</v>
-      </c>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0</v>
-      </c>
-      <c r="F13" s="4">
-        <v>0</v>
-      </c>
-      <c r="G13" s="4">
-        <v>0</v>
-      </c>
-      <c r="H13" s="4">
-        <v>0</v>
-      </c>
-      <c r="I13" s="4">
-        <v>0</v>
-      </c>
-      <c r="J13" s="4">
-        <v>0</v>
-      </c>
-      <c r="K13" s="4">
-        <v>0</v>
-      </c>
-      <c r="L13" s="4">
-        <v>0</v>
-      </c>
-      <c r="M13" s="4">
-        <v>0</v>
-      </c>
-      <c r="N13" s="4">
-        <v>0</v>
-      </c>
-      <c r="O13" s="4">
-        <v>0</v>
-      </c>
-      <c r="P13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="4">
-        <v>0</v>
-      </c>
-      <c r="R13" s="4">
-        <v>0</v>
-      </c>
-      <c r="S13" s="4">
-        <v>0</v>
-      </c>
-      <c r="T13" s="4">
-        <v>0</v>
-      </c>
-      <c r="U13" s="4">
-        <v>0</v>
-      </c>
-      <c r="V13" s="4">
-        <v>0</v>
-      </c>
-      <c r="W13" s="4">
-        <v>0</v>
-      </c>
-      <c r="X13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AF13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AG13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AH13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AI13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AJ13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AK13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AL13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AM13" s="4">
-        <v>0</v>
-      </c>
-      <c r="AN13" s="4">
+      <c r="A13" s="2">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2">
+        <v>0</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>0</v>
+      </c>
+      <c r="G13" s="2">
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0</v>
+      </c>
+      <c r="N13" s="2">
+        <v>0</v>
+      </c>
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="2">
+        <v>0</v>
+      </c>
+      <c r="R13" s="2">
+        <v>0</v>
+      </c>
+      <c r="S13" s="2">
+        <v>0</v>
+      </c>
+      <c r="T13" s="2">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2">
+        <v>1</v>
+      </c>
+      <c r="V13" s="2">
+        <v>1</v>
+      </c>
+      <c r="W13" s="2">
+        <v>1</v>
+      </c>
+      <c r="X13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Y13" s="2">
+        <v>1</v>
+      </c>
+      <c r="Z13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AF13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AG13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AH13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AI13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AJ13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AK13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL13" s="2">
+        <v>1</v>
+      </c>
+      <c r="AM13" s="2">
+        <v>0</v>
+      </c>
+      <c r="AN13" s="2">
         <v>0</v>
       </c>
       <c r="AO13" s="4">
@@ -3422,7 +3427,7 @@
         <v>0</v>
       </c>
       <c r="AB14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC14" s="2">
         <v>0</v>
@@ -3431,7 +3436,7 @@
         <v>0</v>
       </c>
       <c r="AE14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF14" s="2">
         <v>0</v>
@@ -3443,7 +3448,7 @@
         <v>0</v>
       </c>
       <c r="AI14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ14" s="2">
         <v>0</v>
@@ -3452,7 +3457,7 @@
         <v>0</v>
       </c>
       <c r="AL14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM14" s="2">
         <v>0</v>
@@ -3460,7 +3465,7 @@
       <c r="AN14" s="2">
         <v>0</v>
       </c>
-      <c r="AO14" s="2">
+      <c r="AO14" s="4">
         <v>0</v>
       </c>
       <c r="AP14" s="2">
@@ -3543,28 +3548,28 @@
     </row>
     <row r="15" spans="1:112">
       <c r="A15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I15" s="2">
         <v>0</v>
@@ -3624,7 +3629,7 @@
         <v>0</v>
       </c>
       <c r="AB15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC15" s="2">
         <v>0</v>
@@ -3633,7 +3638,7 @@
         <v>0</v>
       </c>
       <c r="AE15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF15" s="2">
         <v>0</v>
@@ -3645,7 +3650,7 @@
         <v>0</v>
       </c>
       <c r="AI15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ15" s="2">
         <v>0</v>
@@ -3654,15 +3659,15 @@
         <v>0</v>
       </c>
       <c r="AL15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN15" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO15" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO15" s="4">
         <v>0</v>
       </c>
       <c r="AP15" s="2">
@@ -3766,58 +3771,58 @@
         <v>0</v>
       </c>
       <c r="H16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z16" s="2">
         <v>0</v>
@@ -3826,7 +3831,7 @@
         <v>0</v>
       </c>
       <c r="AB16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC16" s="2">
         <v>0</v>
@@ -3835,7 +3840,7 @@
         <v>0</v>
       </c>
       <c r="AE16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF16" s="2">
         <v>0</v>
@@ -3847,7 +3852,7 @@
         <v>0</v>
       </c>
       <c r="AI16" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ16" s="2">
         <v>0</v>
@@ -3864,7 +3869,7 @@
       <c r="AN16" s="2">
         <v>0</v>
       </c>
-      <c r="AO16" s="2">
+      <c r="AO16" s="4">
         <v>0</v>
       </c>
       <c r="AP16" s="2">
@@ -4019,7 +4024,7 @@
         <v>0</v>
       </c>
       <c r="Y17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z17" s="2">
         <v>0</v>
@@ -4028,7 +4033,7 @@
         <v>0</v>
       </c>
       <c r="AB17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC17" s="2">
         <v>0</v>
@@ -4037,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="AE17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF17" s="2">
         <v>0</v>
@@ -4049,7 +4054,7 @@
         <v>0</v>
       </c>
       <c r="AI17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ17" s="2">
         <v>0</v>
@@ -4066,7 +4071,7 @@
       <c r="AN17" s="2">
         <v>0</v>
       </c>
-      <c r="AO17" s="2">
+      <c r="AO17" s="4">
         <v>0</v>
       </c>
       <c r="AP17" s="2">
@@ -4149,16 +4154,16 @@
     </row>
     <row r="18" spans="1:100">
       <c r="A18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -4221,7 +4226,7 @@
         <v>0</v>
       </c>
       <c r="Y18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z18" s="2">
         <v>0</v>
@@ -4230,7 +4235,7 @@
         <v>0</v>
       </c>
       <c r="AB18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC18" s="2">
         <v>0</v>
@@ -4239,7 +4244,7 @@
         <v>0</v>
       </c>
       <c r="AE18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF18" s="2">
         <v>0</v>
@@ -4251,7 +4256,7 @@
         <v>0</v>
       </c>
       <c r="AI18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ18" s="2">
         <v>0</v>
@@ -4260,15 +4265,15 @@
         <v>0</v>
       </c>
       <c r="AL18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN18" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO18" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO18" s="4">
         <v>0</v>
       </c>
       <c r="AP18" s="2">
@@ -4360,7 +4365,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2">
         <v>0</v>
@@ -4369,34 +4374,34 @@
         <v>0</v>
       </c>
       <c r="G19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q19" s="2">
         <v>0</v>
@@ -4405,7 +4410,7 @@
         <v>0</v>
       </c>
       <c r="S19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T19" s="2">
         <v>0</v>
@@ -4423,7 +4428,7 @@
         <v>0</v>
       </c>
       <c r="Y19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z19" s="2">
         <v>0</v>
@@ -4432,7 +4437,7 @@
         <v>0</v>
       </c>
       <c r="AB19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC19" s="2">
         <v>0</v>
@@ -4441,19 +4446,19 @@
         <v>0</v>
       </c>
       <c r="AE19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ19" s="2">
         <v>0</v>
@@ -4470,7 +4475,7 @@
       <c r="AN19" s="2">
         <v>0</v>
       </c>
-      <c r="AO19" s="2">
+      <c r="AO19" s="4">
         <v>0</v>
       </c>
       <c r="AP19" s="2">
@@ -4562,7 +4567,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -4580,7 +4585,7 @@
         <v>0</v>
       </c>
       <c r="J20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K20" s="2">
         <v>0</v>
@@ -4598,7 +4603,7 @@
         <v>0</v>
       </c>
       <c r="P20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q20" s="2">
         <v>0</v>
@@ -4607,25 +4612,25 @@
         <v>0</v>
       </c>
       <c r="S20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z20" s="2">
         <v>0</v>
@@ -4634,7 +4639,7 @@
         <v>0</v>
       </c>
       <c r="AB20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC20" s="2">
         <v>0</v>
@@ -4672,7 +4677,7 @@
       <c r="AN20" s="2">
         <v>0</v>
       </c>
-      <c r="AO20" s="2">
+      <c r="AO20" s="4">
         <v>0</v>
       </c>
       <c r="AP20" s="2">
@@ -4764,7 +4769,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2">
         <v>0</v>
@@ -4782,7 +4787,7 @@
         <v>0</v>
       </c>
       <c r="J21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K21" s="2">
         <v>0</v>
@@ -4800,7 +4805,7 @@
         <v>0</v>
       </c>
       <c r="P21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21" s="2">
         <v>0</v>
@@ -4827,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="Y21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z21" s="2">
         <v>0</v>
@@ -4836,7 +4841,7 @@
         <v>0</v>
       </c>
       <c r="AB21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC21" s="2">
         <v>0</v>
@@ -4874,7 +4879,7 @@
       <c r="AN21" s="2">
         <v>0</v>
       </c>
-      <c r="AO21" s="2">
+      <c r="AO21" s="4">
         <v>0</v>
       </c>
       <c r="AP21" s="2">
@@ -4957,16 +4962,16 @@
     </row>
     <row r="22" spans="1:100">
       <c r="A22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2">
         <v>0</v>
@@ -4984,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="J22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" s="2">
         <v>0</v>
@@ -5002,7 +5007,7 @@
         <v>0</v>
       </c>
       <c r="P22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q22" s="2">
         <v>0</v>
@@ -5029,7 +5034,7 @@
         <v>0</v>
       </c>
       <c r="Y22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z22" s="2">
         <v>0</v>
@@ -5038,7 +5043,7 @@
         <v>0</v>
       </c>
       <c r="AB22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC22" s="2">
         <v>0</v>
@@ -5047,36 +5052,36 @@
         <v>0</v>
       </c>
       <c r="AE22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN22" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO22" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO22" s="4">
         <v>0</v>
       </c>
       <c r="AP22" s="2">
@@ -5168,7 +5173,7 @@
         <v>0</v>
       </c>
       <c r="D23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2">
         <v>0</v>
@@ -5186,7 +5191,7 @@
         <v>0</v>
       </c>
       <c r="J23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K23" s="2">
         <v>0</v>
@@ -5195,7 +5200,7 @@
         <v>0</v>
       </c>
       <c r="M23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="2">
         <v>0</v>
@@ -5204,7 +5209,7 @@
         <v>0</v>
       </c>
       <c r="P23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q23" s="2">
         <v>0</v>
@@ -5213,25 +5218,25 @@
         <v>0</v>
       </c>
       <c r="S23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z23" s="2">
         <v>0</v>
@@ -5240,7 +5245,7 @@
         <v>0</v>
       </c>
       <c r="AB23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC23" s="2">
         <v>0</v>
@@ -5249,7 +5254,7 @@
         <v>0</v>
       </c>
       <c r="AE23" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF23" s="2">
         <v>0</v>
@@ -5278,7 +5283,7 @@
       <c r="AN23" s="2">
         <v>0</v>
       </c>
-      <c r="AO23" s="2">
+      <c r="AO23" s="4">
         <v>0</v>
       </c>
       <c r="AP23" s="2">
@@ -5370,16 +5375,16 @@
         <v>0</v>
       </c>
       <c r="D24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H24" s="2">
         <v>0</v>
@@ -5388,7 +5393,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24" s="2">
         <v>0</v>
@@ -5397,7 +5402,7 @@
         <v>0</v>
       </c>
       <c r="M24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N24" s="2">
         <v>0</v>
@@ -5406,7 +5411,7 @@
         <v>0</v>
       </c>
       <c r="P24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q24" s="2">
         <v>0</v>
@@ -5415,7 +5420,7 @@
         <v>0</v>
       </c>
       <c r="S24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" s="2">
         <v>0</v>
@@ -5442,7 +5447,7 @@
         <v>0</v>
       </c>
       <c r="AB24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC24" s="2">
         <v>0</v>
@@ -5451,7 +5456,7 @@
         <v>0</v>
       </c>
       <c r="AE24" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF24" s="2">
         <v>0</v>
@@ -5480,7 +5485,7 @@
       <c r="AN24" s="2">
         <v>0</v>
       </c>
-      <c r="AO24" s="2">
+      <c r="AO24" s="4">
         <v>0</v>
       </c>
       <c r="AP24" s="2">
@@ -5563,16 +5568,16 @@
     </row>
     <row r="25" spans="1:100">
       <c r="A25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E25" s="2">
         <v>0</v>
@@ -5581,7 +5586,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25" s="2">
         <v>0</v>
@@ -5590,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="J25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K25" s="2">
         <v>0</v>
@@ -5599,7 +5604,7 @@
         <v>0</v>
       </c>
       <c r="M25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25" s="2">
         <v>0</v>
@@ -5608,7 +5613,7 @@
         <v>0</v>
       </c>
       <c r="P25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q25" s="2">
         <v>0</v>
@@ -5617,7 +5622,7 @@
         <v>0</v>
       </c>
       <c r="S25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="2">
         <v>0</v>
@@ -5644,7 +5649,7 @@
         <v>0</v>
       </c>
       <c r="AB25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC25" s="2">
         <v>0</v>
@@ -5653,7 +5658,7 @@
         <v>0</v>
       </c>
       <c r="AE25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF25" s="2">
         <v>0</v>
@@ -5662,27 +5667,27 @@
         <v>0</v>
       </c>
       <c r="AH25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM25" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN25" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO25" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO25" s="4">
         <v>0</v>
       </c>
       <c r="AP25" s="2">
@@ -5783,7 +5788,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2">
         <v>0</v>
@@ -5792,7 +5797,7 @@
         <v>0</v>
       </c>
       <c r="J26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K26" s="2">
         <v>0</v>
@@ -5801,7 +5806,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N26" s="2">
         <v>0</v>
@@ -5810,7 +5815,7 @@
         <v>0</v>
       </c>
       <c r="P26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q26" s="2">
         <v>0</v>
@@ -5819,7 +5824,7 @@
         <v>0</v>
       </c>
       <c r="S26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T26" s="2">
         <v>0</v>
@@ -5828,25 +5833,25 @@
         <v>0</v>
       </c>
       <c r="V26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC26" s="2">
         <v>0</v>
@@ -5855,7 +5860,7 @@
         <v>0</v>
       </c>
       <c r="AE26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF26" s="2">
         <v>0</v>
@@ -5864,7 +5869,7 @@
         <v>0</v>
       </c>
       <c r="AH26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI26" s="2">
         <v>0</v>
@@ -5884,7 +5889,7 @@
       <c r="AN26" s="2">
         <v>0</v>
       </c>
-      <c r="AO26" s="2">
+      <c r="AO26" s="4">
         <v>0</v>
       </c>
       <c r="AP26" s="2">
@@ -5985,7 +5990,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="2">
         <v>0</v>
@@ -5994,7 +5999,7 @@
         <v>0</v>
       </c>
       <c r="J27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="2">
         <v>0</v>
@@ -6003,7 +6008,7 @@
         <v>0</v>
       </c>
       <c r="M27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N27" s="2">
         <v>0</v>
@@ -6012,7 +6017,7 @@
         <v>0</v>
       </c>
       <c r="P27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q27" s="2">
         <v>0</v>
@@ -6021,7 +6026,7 @@
         <v>0</v>
       </c>
       <c r="S27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T27" s="2">
         <v>0</v>
@@ -6030,7 +6035,7 @@
         <v>0</v>
       </c>
       <c r="V27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W27" s="2">
         <v>0</v>
@@ -6057,7 +6062,7 @@
         <v>0</v>
       </c>
       <c r="AE27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF27" s="2">
         <v>0</v>
@@ -6066,7 +6071,7 @@
         <v>0</v>
       </c>
       <c r="AH27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI27" s="2">
         <v>0</v>
@@ -6086,7 +6091,7 @@
       <c r="AN27" s="2">
         <v>0</v>
       </c>
-      <c r="AO27" s="2">
+      <c r="AO27" s="4">
         <v>0</v>
       </c>
       <c r="AP27" s="2">
@@ -6169,16 +6174,16 @@
     </row>
     <row r="28" spans="1:100">
       <c r="A28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E28" s="2">
         <v>0</v>
@@ -6187,16 +6192,16 @@
         <v>0</v>
       </c>
       <c r="G28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K28" s="2">
         <v>0</v>
@@ -6205,7 +6210,7 @@
         <v>0</v>
       </c>
       <c r="M28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="2">
         <v>0</v>
@@ -6214,7 +6219,7 @@
         <v>0</v>
       </c>
       <c r="P28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q28" s="2">
         <v>0</v>
@@ -6223,7 +6228,7 @@
         <v>0</v>
       </c>
       <c r="S28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T28" s="2">
         <v>0</v>
@@ -6232,7 +6237,7 @@
         <v>0</v>
       </c>
       <c r="V28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W28" s="2">
         <v>0</v>
@@ -6259,7 +6264,7 @@
         <v>0</v>
       </c>
       <c r="AE28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF28" s="2">
         <v>0</v>
@@ -6268,7 +6273,7 @@
         <v>0</v>
       </c>
       <c r="AH28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI28" s="2">
         <v>0</v>
@@ -6277,18 +6282,18 @@
         <v>0</v>
       </c>
       <c r="AK28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN28" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO28" s="2">
+        <v>1</v>
+      </c>
+      <c r="AO28" s="4">
         <v>0</v>
       </c>
       <c r="AP28" s="2">
@@ -6380,7 +6385,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E29" s="2">
         <v>0</v>
@@ -6407,7 +6412,7 @@
         <v>0</v>
       </c>
       <c r="M29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N29" s="2">
         <v>0</v>
@@ -6416,7 +6421,7 @@
         <v>0</v>
       </c>
       <c r="P29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q29" s="2">
         <v>0</v>
@@ -6425,7 +6430,7 @@
         <v>0</v>
       </c>
       <c r="S29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T29" s="2">
         <v>0</v>
@@ -6434,7 +6439,7 @@
         <v>0</v>
       </c>
       <c r="V29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W29" s="2">
         <v>0</v>
@@ -6452,7 +6457,7 @@
         <v>0</v>
       </c>
       <c r="AB29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC29" s="2">
         <v>0</v>
@@ -6461,7 +6466,7 @@
         <v>0</v>
       </c>
       <c r="AE29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF29" s="2">
         <v>0</v>
@@ -6470,7 +6475,7 @@
         <v>0</v>
       </c>
       <c r="AH29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI29" s="2">
         <v>0</v>
@@ -6479,7 +6484,7 @@
         <v>0</v>
       </c>
       <c r="AK29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL29" s="2">
         <v>0</v>
@@ -6490,7 +6495,7 @@
       <c r="AN29" s="2">
         <v>0</v>
       </c>
-      <c r="AO29" s="2">
+      <c r="AO29" s="4">
         <v>0</v>
       </c>
       <c r="AP29" s="2">
@@ -6582,7 +6587,7 @@
         <v>0</v>
       </c>
       <c r="D30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="2">
         <v>0</v>
@@ -6609,7 +6614,7 @@
         <v>0</v>
       </c>
       <c r="M30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N30" s="2">
         <v>0</v>
@@ -6618,7 +6623,7 @@
         <v>0</v>
       </c>
       <c r="P30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q30" s="2">
         <v>0</v>
@@ -6627,7 +6632,7 @@
         <v>0</v>
       </c>
       <c r="S30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T30" s="2">
         <v>0</v>
@@ -6636,7 +6641,7 @@
         <v>0</v>
       </c>
       <c r="V30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W30" s="2">
         <v>0</v>
@@ -6654,7 +6659,7 @@
         <v>0</v>
       </c>
       <c r="AB30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC30" s="2">
         <v>0</v>
@@ -6663,7 +6668,7 @@
         <v>0</v>
       </c>
       <c r="AE30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF30" s="2">
         <v>0</v>
@@ -6672,7 +6677,7 @@
         <v>0</v>
       </c>
       <c r="AH30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI30" s="2">
         <v>0</v>
@@ -6681,7 +6686,7 @@
         <v>0</v>
       </c>
       <c r="AK30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL30" s="2">
         <v>0</v>
@@ -6692,7 +6697,7 @@
       <c r="AN30" s="2">
         <v>0</v>
       </c>
-      <c r="AO30" s="2">
+      <c r="AO30" s="4">
         <v>0</v>
       </c>
       <c r="AP30" s="2">
@@ -6775,43 +6780,43 @@
     </row>
     <row r="31" spans="1:100">
       <c r="A31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B31" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N31" s="2">
         <v>0</v>
@@ -6820,16 +6825,16 @@
         <v>0</v>
       </c>
       <c r="P31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T31" s="2">
         <v>0</v>
@@ -6838,25 +6843,25 @@
         <v>0</v>
       </c>
       <c r="V31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC31" s="2">
         <v>0</v>
@@ -6865,25 +6870,25 @@
         <v>0</v>
       </c>
       <c r="AE31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AG31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL31" s="2">
         <v>0</v>
@@ -6894,7 +6899,7 @@
       <c r="AN31" s="2">
         <v>0</v>
       </c>
-      <c r="AO31" s="2">
+      <c r="AO31" s="4">
         <v>0</v>
       </c>
       <c r="AP31" s="2">
@@ -6976,127 +6981,127 @@
       <c r="CV31" s="2"/>
     </row>
     <row r="32" spans="1:100">
-      <c r="A32" s="2">
-        <v>0</v>
-      </c>
-      <c r="B32" s="2">
-        <v>0</v>
-      </c>
-      <c r="C32" s="2">
-        <v>0</v>
-      </c>
-      <c r="D32" s="2">
-        <v>0</v>
-      </c>
-      <c r="E32" s="2">
-        <v>0</v>
-      </c>
-      <c r="F32" s="2">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2">
-        <v>0</v>
-      </c>
-      <c r="H32" s="2">
-        <v>0</v>
-      </c>
-      <c r="I32" s="2">
-        <v>0</v>
-      </c>
-      <c r="J32" s="2">
-        <v>0</v>
-      </c>
-      <c r="K32" s="2">
-        <v>0</v>
-      </c>
-      <c r="L32" s="2">
-        <v>0</v>
-      </c>
-      <c r="M32" s="2">
-        <v>0</v>
-      </c>
-      <c r="N32" s="2">
-        <v>0</v>
-      </c>
-      <c r="O32" s="2">
-        <v>0</v>
-      </c>
-      <c r="P32" s="2">
-        <v>0</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>0</v>
-      </c>
-      <c r="R32" s="2">
-        <v>0</v>
-      </c>
-      <c r="S32" s="2">
-        <v>0</v>
-      </c>
-      <c r="T32" s="2">
-        <v>0</v>
-      </c>
-      <c r="U32" s="2">
-        <v>0</v>
-      </c>
-      <c r="V32" s="2">
-        <v>0</v>
-      </c>
-      <c r="W32" s="2">
-        <v>0</v>
-      </c>
-      <c r="X32" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y32" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AA32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AD32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AE32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AF32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AG32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AH32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AI32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AJ32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AK32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AL32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AM32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AN32" s="2">
-        <v>0</v>
-      </c>
-      <c r="AO32" s="2">
+      <c r="A32" s="4">
+        <v>0</v>
+      </c>
+      <c r="B32" s="4">
+        <v>0</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0</v>
+      </c>
+      <c r="E32" s="4">
+        <v>0</v>
+      </c>
+      <c r="F32" s="4">
+        <v>0</v>
+      </c>
+      <c r="G32" s="4">
+        <v>0</v>
+      </c>
+      <c r="H32" s="4">
+        <v>0</v>
+      </c>
+      <c r="I32" s="4">
+        <v>0</v>
+      </c>
+      <c r="J32" s="4">
+        <v>0</v>
+      </c>
+      <c r="K32" s="4">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4">
+        <v>0</v>
+      </c>
+      <c r="M32" s="4">
+        <v>0</v>
+      </c>
+      <c r="N32" s="4">
+        <v>0</v>
+      </c>
+      <c r="O32" s="4">
+        <v>0</v>
+      </c>
+      <c r="P32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="4">
+        <v>0</v>
+      </c>
+      <c r="R32" s="4">
+        <v>0</v>
+      </c>
+      <c r="S32" s="4">
+        <v>0</v>
+      </c>
+      <c r="T32" s="4">
+        <v>0</v>
+      </c>
+      <c r="U32" s="4">
+        <v>0</v>
+      </c>
+      <c r="V32" s="4">
+        <v>0</v>
+      </c>
+      <c r="W32" s="4">
+        <v>0</v>
+      </c>
+      <c r="X32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AI32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN32" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO32" s="4">
         <v>0</v>
       </c>
       <c r="AP32" s="2">
@@ -19009,6 +19014,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="CR25:CV27 CR111:CV112 CW13:DH13">
+    <cfRule type="colorScale" priority="38">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A97:A110 AC97:CQ110">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19018,7 +19033,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A97:A110 AC97:CQ110">
+  <conditionalFormatting sqref="CR97:CV110">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19028,18 +19043,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR97:CV110">
-    <cfRule type="colorScale" priority="35">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="CR56:CV64 CR92:CV96">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -19049,7 +19054,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CR42:CV55">
-    <cfRule type="colorScale" priority="31">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -19059,6 +19064,16 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CR28:CV41">
+    <cfRule type="colorScale" priority="30">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="0"/>
+        <color theme="1" tint="0.249977111117893"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A88:A91 AC88:CQ91">
     <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19068,7 +19083,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A88:A91 AC88:CQ91">
+  <conditionalFormatting sqref="CR88:CV91">
     <cfRule type="colorScale" priority="28">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19078,7 +19093,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR88:CV91">
+  <conditionalFormatting sqref="A83:A87 AC83:CQ87">
     <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19088,7 +19103,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A83:A87 AC83:CQ87">
+  <conditionalFormatting sqref="CR83:CV87">
     <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19098,7 +19113,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR83:CV87">
+  <conditionalFormatting sqref="A79:A82 AC79:CQ82">
     <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19108,7 +19123,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A79:A82 AC79:CQ82">
+  <conditionalFormatting sqref="CR79:CV82">
     <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19118,7 +19133,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR79:CV82">
+  <conditionalFormatting sqref="A74:A78 AC74:CQ78">
     <cfRule type="colorScale" priority="23">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19128,7 +19143,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A74:A78 AC74:CQ78">
+  <conditionalFormatting sqref="CR74:CV78">
     <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19138,7 +19153,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR74:CV78">
+  <conditionalFormatting sqref="A70:A73 AC70:CQ73">
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19148,7 +19163,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A70:A73 AC70:CQ73">
+  <conditionalFormatting sqref="CR70:CV73">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19158,7 +19173,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR70:CV73">
+  <conditionalFormatting sqref="A65:A69 AC65:CQ69">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19168,7 +19183,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A65:A69 AC65:CQ69">
+  <conditionalFormatting sqref="CR65:CV69">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -19178,18 +19193,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="CR65:CV69">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="0"/>
-        <color theme="1" tint="0.249977111117893"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="A2:A6">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -19198,13 +19203,15 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A7:AN12">
+  <conditionalFormatting sqref="A7:AN31">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
-        <color theme="1" tint="0.249977111117893"/>
+        <cfvo type="num" val="2"/>
+        <color theme="1" tint="0.499984740745262"/>
         <color theme="0"/>
+        <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Unknown changes to puzzle near end of development.
</commit_message>
<xml_diff>
--- a/Labyrinth_maze.xlsx
+++ b/Labyrinth_maze.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="0" windowWidth="27320" windowHeight="14820" tabRatio="500"/>
+    <workbookView xWindow="60" yWindow="0" windowWidth="27120" windowHeight="17780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Labyrinth_maze.csv" sheetId="1" r:id="rId1"/>
@@ -679,10 +679,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CV43"/>
+  <dimension ref="A1:AO43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1486,10 +1486,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1608,10 +1608,10 @@
     </row>
     <row r="8" spans="1:41">
       <c r="A8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2">
         <v>1</v>

</xml_diff>